<commit_message>
added image flip to generator
</commit_message>
<xml_diff>
--- a/self-driving-nano/projects/3-behavioral-cloning/results/test-plan.xlsx
+++ b/self-driving-nano/projects/3-behavioral-cloning/results/test-plan.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
   <si>
     <t>TEST</t>
   </si>
@@ -50,12 +50,6 @@
     <t>Turns Completed</t>
   </si>
   <si>
-    <t>LOSS</t>
-  </si>
-  <si>
-    <t>ACC</t>
-  </si>
-  <si>
     <t>EPOCHS</t>
   </si>
   <si>
@@ -104,13 +98,37 @@
     <t>center cam only</t>
   </si>
   <si>
-    <t xml:space="preserve"> + reduce straight angle bias</t>
-  </si>
-  <si>
     <t xml:space="preserve"> + add left and right cams</t>
   </si>
   <si>
     <t xml:space="preserve"> + flip horizontally </t>
+  </si>
+  <si>
+    <t>ipynb</t>
+  </si>
+  <si>
+    <t>v5c</t>
+  </si>
+  <si>
+    <t>VAL ACC</t>
+  </si>
+  <si>
+    <t>VAL LOSS</t>
+  </si>
+  <si>
+    <t>TRAIN LOSS</t>
+  </si>
+  <si>
+    <t>TRAIN ACC</t>
+  </si>
+  <si>
+    <t>v6</t>
+  </si>
+  <si>
+    <t>v7</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> + reduce straight angle bias ??</t>
   </si>
 </sst>
 </file>
@@ -175,7 +193,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -186,6 +204,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -196,6 +220,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
@@ -480,312 +507,352 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K34"/>
+  <dimension ref="A1:N34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="6.5" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" customWidth="1"/>
-    <col min="5" max="5" width="36.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="21.83203125" customWidth="1"/>
-    <col min="9" max="11" width="16.33203125" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" style="10" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="6.5" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" customWidth="1"/>
+    <col min="6" max="6" width="36.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="11.5" style="6" customWidth="1"/>
+    <col min="12" max="14" width="16.33203125" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="5"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="10" t="s">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="7"/>
+      <c r="B1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="10"/>
-      <c r="I1" s="3" t="s">
+      <c r="F1" s="13"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-    </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+    </row>
+    <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="7" t="s">
+      <c r="B2" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="N2" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="8">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="10">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="8">
+        <v>2</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="10">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="6">
+        <v>10</v>
+      </c>
+      <c r="H4" s="6">
+        <v>1.3100000000000001E-2</v>
+      </c>
+      <c r="I4" s="6">
+        <v>0.54139999999999999</v>
+      </c>
+      <c r="J4" s="6">
+        <v>1.2800000000000001E-2</v>
+      </c>
+      <c r="K4" s="6">
+        <v>0.53910000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="8">
+        <v>3</v>
+      </c>
+      <c r="D5" s="10">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="8">
+        <v>4</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="10">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="8">
+        <v>5</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="10">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="8">
+        <v>6</v>
+      </c>
+      <c r="D8" s="10">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="8">
+        <v>7</v>
+      </c>
+      <c r="D9" s="10">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="8">
+        <v>8</v>
+      </c>
+      <c r="D10" s="10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="8">
+        <v>9</v>
+      </c>
+      <c r="D11" s="10">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="4" t="s">
+    </row>
+    <row r="12" spans="1:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="8">
+        <v>10</v>
+      </c>
+      <c r="D12" s="10">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="8">
+        <v>11</v>
+      </c>
+      <c r="D13" s="10">
+        <v>2</v>
+      </c>
+      <c r="E13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="8">
+        <v>12</v>
+      </c>
+      <c r="D14" s="10">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="8">
         <v>13</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="6">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="8">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="D15" s="10">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="8">
         <v>14</v>
       </c>
-      <c r="E3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="6">
+      <c r="D16" s="10">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="8">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="6">
-        <v>3</v>
-      </c>
-      <c r="C5" s="8">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="6">
-        <v>4</v>
-      </c>
-      <c r="C6" s="8">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="6">
-        <v>5</v>
-      </c>
-      <c r="C7" s="8">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="6">
-        <v>6</v>
-      </c>
-      <c r="C8" s="8">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="E16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="8">
+        <v>15</v>
+      </c>
+      <c r="C17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="10">
+        <v>2</v>
+      </c>
+      <c r="E17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="8">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="6">
-        <v>7</v>
-      </c>
-      <c r="C9" s="8">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" t="s">
+    <row r="19" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="8">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="8">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="6">
-        <v>8</v>
-      </c>
-      <c r="C10" s="8">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" t="s">
+    <row r="21" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="8">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="6">
-        <v>9</v>
-      </c>
-      <c r="C11" s="8">
-        <v>1</v>
-      </c>
-      <c r="D11" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="6">
-        <v>10</v>
-      </c>
-      <c r="C12" s="8">
-        <v>1</v>
-      </c>
-      <c r="D12" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="6">
-        <v>11</v>
-      </c>
-      <c r="C13" s="8">
-        <v>2</v>
-      </c>
-      <c r="D13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="6">
-        <v>12</v>
-      </c>
-      <c r="C14" s="8">
-        <v>1</v>
-      </c>
-      <c r="D14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="6">
-        <v>13</v>
-      </c>
-      <c r="C15" s="8">
-        <v>1</v>
-      </c>
-      <c r="D15" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="6">
-        <v>14</v>
-      </c>
-      <c r="C16" s="8">
-        <v>2</v>
-      </c>
-      <c r="D16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="6">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="8">
-        <v>2</v>
-      </c>
-      <c r="D17" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="6">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="6">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="6">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="6">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="34" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="E1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>